<commit_message>
data 20 + Cert
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdolden\Desktop\Ch3_floweringrush\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2D69D2-526E-413A-9C15-A3AA17571CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E46291-7A98-483B-96EE-4F2873610950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="300" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{94130567-C790-4197-BF09-72317C0E58C5}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="32">
   <si>
     <t>High state</t>
   </si>
@@ -244,6 +244,12 @@
     <t>High invasion
 (binned)</t>
   </si>
+  <si>
+    <t>(0.5, 0.75) A + C*</t>
+  </si>
+  <si>
+    <t>C* = assumes perfect citizen science detection</t>
+  </si>
 </sst>
 </file>
 
@@ -331,7 +337,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,8 +368,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="73">
+  <borders count="76">
     <border>
       <left/>
       <right/>
@@ -1245,40 +1257,73 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1287,7 +1332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="237">
+  <cellXfs count="277">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1719,6 +1764,103 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="66" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1759,7 +1901,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1770,6 +1912,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1785,161 +1930,175 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2285,7 +2444,7 @@
   <dimension ref="B1:N74"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="50" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+      <selection activeCell="E14" sqref="E14:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2308,33 +2467,33 @@
       <c r="I1"/>
     </row>
     <row r="2" spans="2:14" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="161" t="s">
+      <c r="E2" s="194" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="162"/>
-      <c r="G2" s="162"/>
-      <c r="H2" s="163"/>
+      <c r="F2" s="195"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="196"/>
       <c r="I2" s="33"/>
-      <c r="J2" s="164" t="s">
+      <c r="J2" s="197" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="162"/>
-      <c r="L2" s="163"/>
+      <c r="K2" s="195"/>
+      <c r="L2" s="196"/>
     </row>
     <row r="3" spans="2:14" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="171" t="s">
+      <c r="B3" s="204" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="172"/>
-      <c r="D3" s="173"/>
-      <c r="E3" s="168" t="s">
+      <c r="C3" s="205"/>
+      <c r="D3" s="206"/>
+      <c r="E3" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="169"/>
-      <c r="G3" s="170" t="s">
+      <c r="F3" s="202"/>
+      <c r="G3" s="203" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="169"/>
+      <c r="H3" s="202"/>
       <c r="I3" s="34"/>
       <c r="J3" s="28" t="s">
         <v>21</v>
@@ -2382,10 +2541,10 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="165" t="s">
+      <c r="B5" s="198" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="233" t="s">
+      <c r="C5" s="207" t="s">
         <v>29</v>
       </c>
       <c r="D5" s="13" t="s">
@@ -2416,8 +2575,8 @@
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="166"/>
-      <c r="C6" s="175"/>
+      <c r="B6" s="199"/>
+      <c r="C6" s="208"/>
       <c r="D6" s="12" t="s">
         <v>9</v>
       </c>
@@ -2434,7 +2593,7 @@
         <v>0.5</v>
       </c>
       <c r="I6" s="37"/>
-      <c r="J6" s="196">
+      <c r="J6" s="176">
         <v>0.23200000000000001</v>
       </c>
       <c r="K6" s="96">
@@ -2446,8 +2605,8 @@
       <c r="M6" s="3"/>
     </row>
     <row r="7" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="166"/>
-      <c r="C7" s="175"/>
+      <c r="B7" s="199"/>
+      <c r="C7" s="208"/>
       <c r="D7" s="13" t="s">
         <v>2</v>
       </c>
@@ -2476,8 +2635,8 @@
       <c r="M7" s="3"/>
     </row>
     <row r="8" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="166"/>
-      <c r="C8" s="175"/>
+      <c r="B8" s="199"/>
+      <c r="C8" s="208"/>
       <c r="D8" s="12" t="s">
         <v>3</v>
       </c>
@@ -2506,18 +2665,18 @@
       <c r="M8" s="3"/>
     </row>
     <row r="9" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="166"/>
-      <c r="C9" s="175"/>
+      <c r="B9" s="199"/>
+      <c r="C9" s="208"/>
       <c r="D9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="190">
+      <c r="E9" s="170">
         <v>0.78200000000000003</v>
       </c>
-      <c r="F9" s="189">
+      <c r="F9" s="169">
         <v>1.38</v>
       </c>
-      <c r="G9" s="188">
+      <c r="G9" s="168">
         <v>0.25700000000000001</v>
       </c>
       <c r="H9" s="126">
@@ -2537,8 +2696,8 @@
       <c r="N9" s="15"/>
     </row>
     <row r="10" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="166"/>
-      <c r="C10" s="176"/>
+      <c r="B10" s="199"/>
+      <c r="C10" s="209"/>
       <c r="D10" s="14" t="s">
         <v>5</v>
       </c>
@@ -2567,8 +2726,8 @@
       <c r="M10" s="3"/>
     </row>
     <row r="11" spans="2:14" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="166"/>
-      <c r="C11" s="177" t="s">
+      <c r="B11" s="199"/>
+      <c r="C11" s="210" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="13" t="s">
@@ -2600,21 +2759,21 @@
       <c r="N11" s="15"/>
     </row>
     <row r="12" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="166"/>
-      <c r="C12" s="175"/>
+      <c r="B12" s="199"/>
+      <c r="C12" s="208"/>
       <c r="D12" s="12" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="70">
         <v>0.63600000000000001</v>
       </c>
-      <c r="F12" s="184">
+      <c r="F12" s="164">
         <v>1.1000000000000001</v>
       </c>
       <c r="G12" s="106">
         <v>0.218</v>
       </c>
-      <c r="H12" s="186">
+      <c r="H12" s="166">
         <v>0.47499999999999998</v>
       </c>
       <c r="I12" s="37"/>
@@ -2624,15 +2783,15 @@
       <c r="K12" s="96">
         <v>-0.65600000000000003</v>
       </c>
-      <c r="L12" s="198">
+      <c r="L12" s="178">
         <v>-8.5300000000000001E-2</v>
       </c>
       <c r="M12" s="5"/>
       <c r="N12" s="15"/>
     </row>
     <row r="13" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="166"/>
-      <c r="C13" s="175"/>
+      <c r="B13" s="199"/>
+      <c r="C13" s="208"/>
       <c r="D13" s="13" t="s">
         <v>2</v>
       </c>
@@ -2662,28 +2821,28 @@
       <c r="N13" s="15"/>
     </row>
     <row r="14" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="166"/>
-      <c r="C14" s="175"/>
+      <c r="B14" s="199"/>
+      <c r="C14" s="208"/>
       <c r="D14" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="183">
+      <c r="E14" s="163">
         <v>0.61799999999999999</v>
       </c>
       <c r="F14" s="85">
         <v>1.1200000000000001</v>
       </c>
-      <c r="G14" s="185">
+      <c r="G14" s="165">
         <v>0.21099999999999999</v>
       </c>
-      <c r="H14" s="187">
+      <c r="H14" s="167">
         <v>0.47499999999999998</v>
       </c>
       <c r="I14" s="40"/>
       <c r="J14" s="97">
         <v>0.16700000000000001</v>
       </c>
-      <c r="K14" s="197">
+      <c r="K14" s="177">
         <v>-0.89800000000000002</v>
       </c>
       <c r="L14" s="102">
@@ -2693,8 +2852,8 @@
       <c r="N14" s="15"/>
     </row>
     <row r="15" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="166"/>
-      <c r="C15" s="175"/>
+      <c r="B15" s="199"/>
+      <c r="C15" s="208"/>
       <c r="D15" s="12" t="s">
         <v>4</v>
       </c>
@@ -2704,27 +2863,27 @@
       <c r="F15" s="69">
         <v>1.27</v>
       </c>
-      <c r="G15" s="188">
+      <c r="G15" s="168">
         <v>0.25700000000000001</v>
       </c>
-      <c r="H15" s="191">
+      <c r="H15" s="171">
         <v>0.57499999999999996</v>
       </c>
       <c r="I15" s="40"/>
-      <c r="J15" s="192">
+      <c r="J15" s="172">
         <v>0.13</v>
       </c>
       <c r="K15" s="97">
         <v>0.14399999999999999</v>
       </c>
-      <c r="L15" s="194">
+      <c r="L15" s="174">
         <v>-6.2899999999999998E-2</v>
       </c>
       <c r="M15" s="3"/>
     </row>
     <row r="16" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="166"/>
-      <c r="C16" s="176"/>
+      <c r="B16" s="199"/>
+      <c r="C16" s="209"/>
       <c r="D16" s="14" t="s">
         <v>5</v>
       </c>
@@ -2744,10 +2903,10 @@
       <c r="J16" s="103">
         <v>0.13500000000000001</v>
       </c>
-      <c r="K16" s="193">
+      <c r="K16" s="173">
         <v>1.7299999999999999E-2</v>
       </c>
-      <c r="L16" s="195">
+      <c r="L16" s="175">
         <v>-6.25E-2</v>
       </c>
       <c r="M16" s="3"/>
@@ -2766,10 +2925,10 @@
       <c r="L17" s="24"/>
     </row>
     <row r="18" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="165" t="s">
+      <c r="B18" s="198" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="174" t="s">
+      <c r="C18" s="211" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="50" t="s">
@@ -2785,8 +2944,8 @@
       <c r="L18" s="95"/>
     </row>
     <row r="19" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="166"/>
-      <c r="C19" s="175"/>
+      <c r="B19" s="199"/>
+      <c r="C19" s="208"/>
       <c r="D19" s="49" t="s">
         <v>9</v>
       </c>
@@ -2800,8 +2959,8 @@
       <c r="L19" s="96"/>
     </row>
     <row r="20" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="166"/>
-      <c r="C20" s="175"/>
+      <c r="B20" s="199"/>
+      <c r="C20" s="208"/>
       <c r="D20" s="49" t="s">
         <v>2</v>
       </c>
@@ -2815,8 +2974,8 @@
       <c r="L20" s="97"/>
     </row>
     <row r="21" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="166"/>
-      <c r="C21" s="175"/>
+      <c r="B21" s="199"/>
+      <c r="C21" s="208"/>
       <c r="D21" s="13" t="s">
         <v>3</v>
       </c>
@@ -2830,8 +2989,8 @@
       <c r="L21" s="97"/>
     </row>
     <row r="22" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="166"/>
-      <c r="C22" s="175"/>
+      <c r="B22" s="199"/>
+      <c r="C22" s="208"/>
       <c r="D22" s="12" t="s">
         <v>4</v>
       </c>
@@ -2845,8 +3004,8 @@
       <c r="L22" s="97"/>
     </row>
     <row r="23" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="166"/>
-      <c r="C23" s="176"/>
+      <c r="B23" s="199"/>
+      <c r="C23" s="209"/>
       <c r="D23" s="14" t="s">
         <v>5</v>
       </c>
@@ -2860,8 +3019,8 @@
       <c r="L23" s="98"/>
     </row>
     <row r="24" spans="2:14" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="166"/>
-      <c r="C24" s="177" t="s">
+      <c r="B24" s="199"/>
+      <c r="C24" s="210" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="13" t="s">
@@ -2879,8 +3038,8 @@
       <c r="N24" s="15"/>
     </row>
     <row r="25" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="166"/>
-      <c r="C25" s="175"/>
+      <c r="B25" s="199"/>
+      <c r="C25" s="208"/>
       <c r="D25" s="12" t="s">
         <v>9</v>
       </c>
@@ -2894,8 +3053,8 @@
       <c r="L25" s="96"/>
     </row>
     <row r="26" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="166"/>
-      <c r="C26" s="175"/>
+      <c r="B26" s="199"/>
+      <c r="C26" s="208"/>
       <c r="D26" s="13" t="s">
         <v>2</v>
       </c>
@@ -2910,8 +3069,8 @@
       <c r="M26" s="15"/>
     </row>
     <row r="27" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="166"/>
-      <c r="C27" s="175"/>
+      <c r="B27" s="199"/>
+      <c r="C27" s="208"/>
       <c r="D27" s="12" t="s">
         <v>3</v>
       </c>
@@ -2926,8 +3085,8 @@
       <c r="N27" s="15"/>
     </row>
     <row r="28" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="166"/>
-      <c r="C28" s="175"/>
+      <c r="B28" s="199"/>
+      <c r="C28" s="208"/>
       <c r="D28" s="12" t="s">
         <v>4</v>
       </c>
@@ -2941,8 +3100,8 @@
       <c r="L28" s="97"/>
     </row>
     <row r="29" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="166"/>
-      <c r="C29" s="176"/>
+      <c r="B29" s="199"/>
+      <c r="C29" s="209"/>
       <c r="D29" s="14" t="s">
         <v>5</v>
       </c>
@@ -2969,10 +3128,10 @@
       <c r="L30" s="21"/>
     </row>
     <row r="31" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="165" t="s">
+      <c r="B31" s="198" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="174" t="s">
+      <c r="C31" s="211" t="s">
         <v>0</v>
       </c>
       <c r="D31" s="25" t="s">
@@ -2988,8 +3147,8 @@
       <c r="L31" s="123"/>
     </row>
     <row r="32" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="166"/>
-      <c r="C32" s="175"/>
+      <c r="B32" s="199"/>
+      <c r="C32" s="208"/>
       <c r="D32" s="7" t="s">
         <v>9</v>
       </c>
@@ -3003,8 +3162,8 @@
       <c r="L32" s="85"/>
     </row>
     <row r="33" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="166"/>
-      <c r="C33" s="175"/>
+      <c r="B33" s="199"/>
+      <c r="C33" s="208"/>
       <c r="D33" s="8" t="s">
         <v>2</v>
       </c>
@@ -3018,8 +3177,8 @@
       <c r="L33" s="124"/>
     </row>
     <row r="34" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="166"/>
-      <c r="C34" s="175"/>
+      <c r="B34" s="199"/>
+      <c r="C34" s="208"/>
       <c r="D34" s="7" t="s">
         <v>3</v>
       </c>
@@ -3033,8 +3192,8 @@
       <c r="L34" s="125"/>
     </row>
     <row r="35" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="166"/>
-      <c r="C35" s="175"/>
+      <c r="B35" s="199"/>
+      <c r="C35" s="208"/>
       <c r="D35" s="7" t="s">
         <v>4</v>
       </c>
@@ -3048,8 +3207,8 @@
       <c r="L35" s="125"/>
     </row>
     <row r="36" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="166"/>
-      <c r="C36" s="176"/>
+      <c r="B36" s="199"/>
+      <c r="C36" s="209"/>
       <c r="D36" s="9" t="s">
         <v>5</v>
       </c>
@@ -3063,8 +3222,8 @@
       <c r="L36" s="127"/>
     </row>
     <row r="37" spans="2:14" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="166"/>
-      <c r="C37" s="177" t="s">
+      <c r="B37" s="199"/>
+      <c r="C37" s="210" t="s">
         <v>1</v>
       </c>
       <c r="D37" s="8" t="s">
@@ -3080,8 +3239,8 @@
       <c r="L37" s="81"/>
     </row>
     <row r="38" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="166"/>
-      <c r="C38" s="175"/>
+      <c r="B38" s="199"/>
+      <c r="C38" s="208"/>
       <c r="D38" s="7" t="s">
         <v>9</v>
       </c>
@@ -3095,8 +3254,8 @@
       <c r="L38" s="85"/>
     </row>
     <row r="39" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="166"/>
-      <c r="C39" s="175"/>
+      <c r="B39" s="199"/>
+      <c r="C39" s="208"/>
       <c r="D39" s="8" t="s">
         <v>2</v>
       </c>
@@ -3111,8 +3270,8 @@
       <c r="N39" s="15"/>
     </row>
     <row r="40" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="166"/>
-      <c r="C40" s="175"/>
+      <c r="B40" s="199"/>
+      <c r="C40" s="208"/>
       <c r="D40" s="7" t="s">
         <v>3</v>
       </c>
@@ -3126,8 +3285,8 @@
       <c r="L40" s="125"/>
     </row>
     <row r="41" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="166"/>
-      <c r="C41" s="175"/>
+      <c r="B41" s="199"/>
+      <c r="C41" s="208"/>
       <c r="D41" s="7" t="s">
         <v>4</v>
       </c>
@@ -3142,8 +3301,8 @@
       <c r="N41" s="15"/>
     </row>
     <row r="42" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="167"/>
-      <c r="C42" s="178"/>
+      <c r="B42" s="200"/>
+      <c r="C42" s="212"/>
       <c r="D42" s="22" t="s">
         <v>5</v>
       </c>
@@ -3276,10 +3435,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5764096-CBDC-48A7-984B-BFD813F170CD}">
-  <dimension ref="B1:N31"/>
+  <dimension ref="B1:V33"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" zoomScaleSheetLayoutView="50" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C7"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3287,7 +3446,7 @@
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" customWidth="1"/>
     <col min="6" max="6" width="6.28515625" customWidth="1"/>
     <col min="7" max="7" width="6.85546875" customWidth="1"/>
@@ -3296,7 +3455,7 @@
     <col min="10" max="11" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:22" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
       <c r="D1" s="53"/>
@@ -3306,7 +3465,7 @@
       <c r="H1" s="56"/>
       <c r="I1" s="59"/>
     </row>
-    <row r="2" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:22" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2"/>
@@ -3315,36 +3474,36 @@
       <c r="G2"/>
       <c r="H2"/>
     </row>
-    <row r="3" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:22" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3"/>
       <c r="C3"/>
       <c r="D3"/>
-      <c r="E3" s="161" t="s">
+      <c r="E3" s="194" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="162"/>
-      <c r="G3" s="162"/>
-      <c r="H3" s="163"/>
-      <c r="I3" s="164" t="s">
+      <c r="F3" s="195"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="196"/>
+      <c r="I3" s="197" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="162"/>
-      <c r="K3" s="163"/>
-    </row>
-    <row r="4" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="171" t="s">
+      <c r="J3" s="195"/>
+      <c r="K3" s="196"/>
+    </row>
+    <row r="4" spans="2:22" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="204" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="172"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="168" t="s">
+      <c r="C4" s="205"/>
+      <c r="D4" s="206"/>
+      <c r="E4" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="169"/>
-      <c r="G4" s="170" t="s">
+      <c r="F4" s="202"/>
+      <c r="G4" s="203" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="169"/>
+      <c r="H4" s="202"/>
       <c r="I4" s="28" t="s">
         <v>21</v>
       </c>
@@ -3355,334 +3514,416 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="235" t="s">
+    <row r="5" spans="2:22" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="193" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="234" t="s">
+      <c r="C5" s="192" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="220" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="221" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="222" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="222" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="220" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="223" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="223" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="179" t="s">
+    <row r="6" spans="2:22" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="219" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="181" t="s">
+      <c r="C6" s="217" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="225" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="132">
+      <c r="E6" s="226">
         <v>0.63800000000000001</v>
       </c>
-      <c r="F6" s="212">
+      <c r="F6" s="242">
         <v>1.18</v>
       </c>
-      <c r="G6" s="110">
+      <c r="G6" s="254">
         <v>0.217</v>
       </c>
-      <c r="H6" s="213">
+      <c r="H6" s="238">
         <v>0.5</v>
       </c>
-      <c r="I6" s="230">
+      <c r="I6" s="273">
         <v>0.16600000000000001</v>
       </c>
-      <c r="J6" s="108">
+      <c r="J6" s="255">
         <v>-0.58899999999999997</v>
       </c>
-      <c r="K6" s="232">
+      <c r="K6" s="256">
         <v>-7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="180"/>
-      <c r="C7" s="182"/>
-      <c r="D7" s="52" t="s">
+    <row r="7" spans="2:22" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="213"/>
+      <c r="C7" s="218"/>
+      <c r="D7" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="210">
+      <c r="E7" s="224">
         <v>0.63600000000000001</v>
       </c>
-      <c r="F7" s="141">
+      <c r="F7" s="239">
         <v>1.3</v>
       </c>
-      <c r="G7" s="211">
+      <c r="G7" s="224">
         <v>0.21299999999999999</v>
       </c>
-      <c r="H7" s="214">
+      <c r="H7" s="239">
         <v>0.5</v>
       </c>
-      <c r="I7" s="208">
+      <c r="I7" s="257">
         <v>0.216</v>
       </c>
-      <c r="J7" s="231">
+      <c r="J7" s="274">
         <v>1.4E-2</v>
       </c>
-      <c r="K7" s="209">
+      <c r="K7" s="258">
         <v>-0.12</v>
       </c>
     </row>
-    <row r="8" spans="2:13" s="57" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="152"/>
-      <c r="C8" s="153"/>
-      <c r="D8" s="154"/>
-      <c r="E8" s="155"/>
-      <c r="F8" s="156"/>
-      <c r="G8" s="157"/>
-      <c r="H8" s="206"/>
-      <c r="I8" s="158"/>
-      <c r="J8" s="159"/>
-      <c r="K8" s="160"/>
-    </row>
-    <row r="9" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="179" t="s">
+    <row r="8" spans="2:22" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="213"/>
+      <c r="C8" s="231"/>
+      <c r="D8" s="232" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="233">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="F8" s="261">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="G8" s="233">
+        <v>0.22</v>
+      </c>
+      <c r="H8" s="240">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="247">
+        <v>0.217</v>
+      </c>
+      <c r="J8" s="247">
+        <v>-0.219</v>
+      </c>
+      <c r="K8" s="253">
+        <v>-0.16</v>
+      </c>
+      <c r="L8" s="230" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" s="57" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="161"/>
+      <c r="C9" s="162" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="225" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="259">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="F9" s="262">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="G9" s="260">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="H9" s="263">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="I9" s="248">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="J9" s="252">
+        <v>-0.89800000000000002</v>
+      </c>
+      <c r="K9" s="275">
+        <v>-6.6000000000000003E-2</v>
+      </c>
+      <c r="L9" s="230"/>
+      <c r="M9" s="234"/>
+      <c r="N9" s="234"/>
+      <c r="O9" s="234"/>
+      <c r="P9" s="234"/>
+      <c r="Q9" s="234"/>
+      <c r="R9" s="234"/>
+      <c r="S9" s="234"/>
+      <c r="T9" s="234"/>
+      <c r="U9" s="234"/>
+      <c r="V9" s="234"/>
+    </row>
+    <row r="10" spans="2:22" s="57" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="152"/>
+      <c r="C10" s="153"/>
+      <c r="D10" s="154"/>
+      <c r="E10" s="155"/>
+      <c r="F10" s="156"/>
+      <c r="G10" s="157"/>
+      <c r="H10" s="182"/>
+      <c r="I10" s="158"/>
+      <c r="J10" s="159"/>
+      <c r="K10" s="160"/>
+      <c r="M10" s="234"/>
+      <c r="N10" s="234"/>
+      <c r="O10" s="234"/>
+      <c r="P10" s="234"/>
+      <c r="Q10" s="234"/>
+      <c r="R10" s="234"/>
+      <c r="S10" s="234"/>
+      <c r="T10" s="234"/>
+      <c r="U10" s="234"/>
+      <c r="V10" s="234"/>
+    </row>
+    <row r="11" spans="2:22" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="213" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="181" t="s">
+      <c r="C11" s="215" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="130"/>
-      <c r="F9" s="131"/>
-      <c r="G9" s="139"/>
-      <c r="H9" s="207"/>
-      <c r="I9" s="149"/>
-      <c r="J9" s="150"/>
-      <c r="K9" s="151"/>
-      <c r="L9" s="61"/>
-      <c r="M9"/>
-    </row>
-    <row r="10" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="180"/>
-      <c r="C10" s="182"/>
-      <c r="D10" s="52" t="s">
+      <c r="E11" s="130"/>
+      <c r="F11" s="131"/>
+      <c r="G11" s="139"/>
+      <c r="H11" s="183"/>
+      <c r="I11" s="149"/>
+      <c r="J11" s="150"/>
+      <c r="K11" s="151"/>
+      <c r="L11" s="61"/>
+      <c r="M11" s="234"/>
+      <c r="N11" s="235"/>
+      <c r="O11" s="235"/>
+      <c r="P11" s="236"/>
+      <c r="Q11" s="237"/>
+      <c r="R11" s="237"/>
+      <c r="S11" s="236"/>
+      <c r="T11" s="236"/>
+      <c r="U11" s="237"/>
+      <c r="V11" s="234"/>
+    </row>
+    <row r="12" spans="2:22" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="214"/>
+      <c r="C12" s="216"/>
+      <c r="D12" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="140"/>
-      <c r="F10" s="141"/>
-      <c r="G10" s="142"/>
-      <c r="H10" s="205"/>
-      <c r="I10" s="143"/>
-      <c r="J10" s="144"/>
-      <c r="K10" s="145"/>
-      <c r="L10" s="61"/>
-      <c r="M10"/>
-    </row>
-    <row r="11" spans="2:13" s="57" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="152"/>
-      <c r="C11" s="153"/>
-      <c r="D11" s="154"/>
-      <c r="E11" s="155"/>
-      <c r="F11" s="156"/>
-      <c r="G11" s="157"/>
-      <c r="H11" s="206"/>
-      <c r="I11" s="158"/>
-      <c r="J11" s="159"/>
-      <c r="K11" s="160"/>
-      <c r="L11" s="61"/>
-      <c r="M11"/>
-    </row>
-    <row r="12" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="179" t="s">
+      <c r="E12" s="140"/>
+      <c r="F12" s="141"/>
+      <c r="G12" s="142"/>
+      <c r="H12" s="181"/>
+      <c r="I12" s="143"/>
+      <c r="J12" s="144"/>
+      <c r="K12" s="145"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="234"/>
+      <c r="N12" s="234"/>
+      <c r="O12" s="234"/>
+      <c r="P12" s="234"/>
+      <c r="Q12" s="234"/>
+      <c r="R12" s="234"/>
+      <c r="S12" s="234"/>
+      <c r="T12" s="234"/>
+      <c r="U12" s="234"/>
+      <c r="V12" s="234"/>
+    </row>
+    <row r="13" spans="2:22" s="57" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="152"/>
+      <c r="C13" s="153"/>
+      <c r="D13" s="154"/>
+      <c r="E13" s="155"/>
+      <c r="F13" s="156"/>
+      <c r="G13" s="157"/>
+      <c r="H13" s="182"/>
+      <c r="I13" s="158"/>
+      <c r="J13" s="159"/>
+      <c r="K13" s="160"/>
+      <c r="L13" s="61"/>
+      <c r="M13"/>
+    </row>
+    <row r="14" spans="2:22" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="213" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="181" t="s">
+      <c r="C14" s="215" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D14" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="130"/>
-      <c r="F12" s="131"/>
-      <c r="G12" s="139"/>
-      <c r="H12" s="207"/>
-      <c r="I12" s="146"/>
-      <c r="J12" s="147"/>
-      <c r="K12" s="148"/>
-      <c r="L12"/>
-      <c r="M12"/>
-    </row>
-    <row r="13" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="180"/>
-      <c r="C13" s="182"/>
-      <c r="D13" s="52" t="s">
+      <c r="E14" s="130"/>
+      <c r="F14" s="131"/>
+      <c r="G14" s="139"/>
+      <c r="H14" s="183"/>
+      <c r="I14" s="146"/>
+      <c r="J14" s="147"/>
+      <c r="K14" s="148"/>
+      <c r="L14"/>
+      <c r="M14"/>
+    </row>
+    <row r="15" spans="2:22" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="214"/>
+      <c r="C15" s="216"/>
+      <c r="D15" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="140"/>
-      <c r="F13" s="141"/>
-      <c r="G13" s="142"/>
-      <c r="H13" s="205"/>
-      <c r="I13" s="143"/>
-      <c r="J13" s="144"/>
-      <c r="K13" s="145"/>
-      <c r="L13"/>
-      <c r="M13"/>
-    </row>
-    <row r="14" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="58"/>
-    </row>
-    <row r="15" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="56"/>
-    </row>
-    <row r="16" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="140"/>
+      <c r="F15" s="141"/>
+      <c r="G15" s="142"/>
+      <c r="H15" s="181"/>
+      <c r="I15" s="143"/>
+      <c r="J15" s="144"/>
+      <c r="K15" s="145"/>
+      <c r="L15"/>
+      <c r="M15"/>
+    </row>
+    <row r="16" spans="2:22" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="60"/>
       <c r="C16" s="60"/>
       <c r="D16" s="53"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
     </row>
     <row r="17" spans="2:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="60"/>
       <c r="C17" s="60"/>
       <c r="D17" s="53"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="56"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="58"/>
       <c r="H17" s="56"/>
     </row>
     <row r="18" spans="2:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="60"/>
       <c r="C18" s="60"/>
       <c r="D18" s="53"/>
-      <c r="E18" s="58"/>
+      <c r="E18" s="56"/>
       <c r="F18" s="56"/>
-      <c r="G18" s="58"/>
+      <c r="G18" s="56"/>
       <c r="H18" s="56"/>
-      <c r="I18" s="59"/>
     </row>
     <row r="19" spans="2:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="60"/>
       <c r="C19" s="60"/>
       <c r="D19" s="53"/>
-      <c r="E19" s="199"/>
-      <c r="F19" s="200"/>
-      <c r="G19" s="201"/>
-      <c r="H19" s="202"/>
-      <c r="I19" s="203"/>
-      <c r="J19" s="203"/>
-      <c r="K19" s="203"/>
-      <c r="L19" s="203"/>
-      <c r="M19" s="203"/>
-      <c r="N19" s="203"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="56"/>
     </row>
     <row r="20" spans="2:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="60"/>
       <c r="C20" s="60"/>
       <c r="D20" s="53"/>
-      <c r="E20" s="200"/>
-      <c r="F20" s="200"/>
-      <c r="G20" s="201"/>
-      <c r="H20" s="202"/>
-      <c r="I20" s="204"/>
-      <c r="J20" s="203"/>
-      <c r="K20" s="203"/>
-      <c r="L20" s="203"/>
-      <c r="M20" s="203"/>
-      <c r="N20" s="203"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="59"/>
     </row>
     <row r="21" spans="2:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="60"/>
       <c r="C21" s="60"/>
       <c r="D21" s="53"/>
-      <c r="E21" s="199"/>
-      <c r="F21" s="200"/>
-      <c r="G21" s="200"/>
-      <c r="H21" s="201"/>
-      <c r="I21" s="202"/>
-      <c r="J21" s="202"/>
-      <c r="K21" s="201"/>
-      <c r="L21" s="201"/>
-      <c r="M21" s="201"/>
-      <c r="N21" s="203"/>
+      <c r="E21" s="179"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="112"/>
+      <c r="H21" s="180"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
     </row>
     <row r="22" spans="2:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="60"/>
       <c r="C22" s="60"/>
       <c r="D22" s="53"/>
-      <c r="E22" s="199"/>
-      <c r="F22" s="200"/>
-      <c r="G22" s="202"/>
-      <c r="H22" s="202"/>
-      <c r="I22" s="203"/>
-      <c r="J22" s="203"/>
-      <c r="K22" s="203"/>
-      <c r="L22" s="203"/>
-      <c r="M22" s="203"/>
-      <c r="N22" s="203"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="112"/>
+      <c r="H22" s="180"/>
+      <c r="I22" s="15"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
     </row>
     <row r="23" spans="2:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="60"/>
       <c r="C23" s="60"/>
       <c r="D23" s="53"/>
-      <c r="E23" s="199"/>
-      <c r="F23" s="200"/>
-      <c r="G23" s="202"/>
-      <c r="H23" s="202"/>
-      <c r="I23" s="203"/>
-      <c r="J23" s="203"/>
-      <c r="K23" s="203"/>
-      <c r="L23" s="203"/>
-      <c r="M23" s="203"/>
-      <c r="N23" s="203"/>
+      <c r="E23" s="179"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="112"/>
+      <c r="I23" s="180"/>
+      <c r="J23" s="180"/>
+      <c r="K23" s="112"/>
+      <c r="L23" s="112"/>
+      <c r="M23" s="112"/>
+      <c r="N23"/>
     </row>
     <row r="24" spans="2:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="60"/>
       <c r="C24" s="60"/>
       <c r="D24" s="53"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="56"/>
+      <c r="E24" s="179"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="180"/>
+      <c r="H24" s="180"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
     </row>
     <row r="25" spans="2:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="60"/>
       <c r="C25" s="60"/>
       <c r="D25" s="53"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="56"/>
+      <c r="E25" s="179"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="180"/>
+      <c r="H25" s="180"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
     </row>
     <row r="26" spans="2:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="60"/>
@@ -3691,7 +3932,7 @@
       <c r="E26" s="54"/>
       <c r="F26" s="55"/>
       <c r="G26" s="58"/>
-      <c r="H26" s="58"/>
+      <c r="H26" s="56"/>
     </row>
     <row r="27" spans="2:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="60"/>
@@ -3702,23 +3943,41 @@
       <c r="G27" s="58"/>
       <c r="H27" s="56"/>
     </row>
-    <row r="28" spans="2:14" s="57" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:14" s="57" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="60"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="58"/>
+    </row>
+    <row r="29" spans="2:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="60"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="56"/>
+    </row>
     <row r="30" spans="2:14" s="57" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="2:14" s="57" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:14" s="57" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="57" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
     <mergeCell ref="I3:K3"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B6:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3730,7 +3989,7 @@
   <dimension ref="B1:N74"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3754,33 +4013,33 @@
       <c r="I1"/>
     </row>
     <row r="2" spans="2:14" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="161" t="s">
+      <c r="E2" s="194" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="162"/>
-      <c r="G2" s="162"/>
-      <c r="H2" s="163"/>
+      <c r="F2" s="195"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="196"/>
       <c r="I2" s="33"/>
-      <c r="J2" s="164" t="s">
+      <c r="J2" s="197" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="162"/>
-      <c r="L2" s="163"/>
+      <c r="K2" s="195"/>
+      <c r="L2" s="196"/>
     </row>
     <row r="3" spans="2:14" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="171" t="s">
+      <c r="B3" s="204" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="172"/>
-      <c r="D3" s="173"/>
-      <c r="E3" s="168" t="s">
+      <c r="C3" s="205"/>
+      <c r="D3" s="206"/>
+      <c r="E3" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="169"/>
-      <c r="G3" s="170" t="s">
+      <c r="F3" s="202"/>
+      <c r="G3" s="203" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="169"/>
+      <c r="H3" s="202"/>
       <c r="I3" s="34"/>
       <c r="J3" s="28" t="s">
         <v>21</v>
@@ -3828,10 +4087,10 @@
       <c r="M4" s="1"/>
     </row>
     <row r="5" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="165" t="s">
+      <c r="B5" s="198" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="233" t="s">
+      <c r="C5" s="207" t="s">
         <v>29</v>
       </c>
       <c r="D5" s="13" t="s">
@@ -3862,8 +4121,8 @@
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="166"/>
-      <c r="C6" s="175"/>
+      <c r="B6" s="199"/>
+      <c r="C6" s="208"/>
       <c r="D6" s="12" t="s">
         <v>9</v>
       </c>
@@ -3883,7 +4142,7 @@
       <c r="J6" s="96">
         <v>0.22800000000000001</v>
       </c>
-      <c r="K6" s="196">
+      <c r="K6" s="176">
         <v>-0.876</v>
       </c>
       <c r="L6" s="90">
@@ -3893,8 +4152,8 @@
       <c r="N6" s="15"/>
     </row>
     <row r="7" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="166"/>
-      <c r="C7" s="175"/>
+      <c r="B7" s="199"/>
+      <c r="C7" s="208"/>
       <c r="D7" s="13" t="s">
         <v>2</v>
       </c>
@@ -3924,8 +4183,8 @@
       <c r="N7" s="15"/>
     </row>
     <row r="8" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="166"/>
-      <c r="C8" s="175"/>
+      <c r="B8" s="199"/>
+      <c r="C8" s="208"/>
       <c r="D8" s="12" t="s">
         <v>3</v>
       </c>
@@ -3954,25 +4213,25 @@
       <c r="M8" s="3"/>
     </row>
     <row r="9" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="166"/>
-      <c r="C9" s="175"/>
+      <c r="B9" s="199"/>
+      <c r="C9" s="208"/>
       <c r="D9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="190">
+      <c r="E9" s="170">
         <v>0.78400000000000003</v>
       </c>
-      <c r="F9" s="189">
+      <c r="F9" s="169">
         <v>1.42</v>
       </c>
-      <c r="G9" s="188">
+      <c r="G9" s="168">
         <v>0.26200000000000001</v>
       </c>
-      <c r="H9" s="219">
+      <c r="H9" s="188">
         <v>0.65</v>
       </c>
       <c r="I9" s="38"/>
-      <c r="J9" s="192">
+      <c r="J9" s="172">
         <v>0.13</v>
       </c>
       <c r="K9" s="97">
@@ -3984,21 +4243,21 @@
       <c r="M9" s="2"/>
     </row>
     <row r="10" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="166"/>
-      <c r="C10" s="176"/>
+      <c r="B10" s="199"/>
+      <c r="C10" s="209"/>
       <c r="D10" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="133">
         <v>0.68500000000000005</v>
       </c>
-      <c r="F10" s="216">
+      <c r="F10" s="185">
         <v>1.02</v>
       </c>
       <c r="G10" s="113">
         <v>0.224</v>
       </c>
-      <c r="H10" s="217">
+      <c r="H10" s="186">
         <v>0.4</v>
       </c>
       <c r="I10" s="39"/>
@@ -4014,8 +4273,8 @@
       <c r="M10" s="3"/>
     </row>
     <row r="11" spans="2:14" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="166"/>
-      <c r="C11" s="177" t="s">
+      <c r="B11" s="199"/>
+      <c r="C11" s="210" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="13" t="s">
@@ -4034,7 +4293,7 @@
         <v>0.47499999999999998</v>
       </c>
       <c r="I11" s="36"/>
-      <c r="J11" s="218">
+      <c r="J11" s="187">
         <v>0.23100000000000001</v>
       </c>
       <c r="K11" s="100">
@@ -4047,8 +4306,8 @@
       <c r="N11" s="15"/>
     </row>
     <row r="12" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="166"/>
-      <c r="C12" s="175"/>
+      <c r="B12" s="199"/>
+      <c r="C12" s="208"/>
       <c r="D12" s="12" t="s">
         <v>9</v>
       </c>
@@ -4071,15 +4330,15 @@
       <c r="K12" s="96">
         <v>-0.82199999999999995</v>
       </c>
-      <c r="L12" s="198">
+      <c r="L12" s="178">
         <v>-6.7299999999999999E-2</v>
       </c>
-      <c r="M12" s="215"/>
+      <c r="M12" s="184"/>
       <c r="N12" s="15"/>
     </row>
     <row r="13" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="166"/>
-      <c r="C13" s="175"/>
+      <c r="B13" s="199"/>
+      <c r="C13" s="208"/>
       <c r="D13" s="13" t="s">
         <v>2</v>
       </c>
@@ -4109,18 +4368,18 @@
       <c r="N13" s="15"/>
     </row>
     <row r="14" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="166"/>
-      <c r="C14" s="175"/>
+      <c r="B14" s="199"/>
+      <c r="C14" s="208"/>
       <c r="D14" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="183">
+      <c r="E14" s="163">
         <v>0.61199999999999999</v>
       </c>
       <c r="F14" s="85">
         <v>1.1499999999999999</v>
       </c>
-      <c r="G14" s="185">
+      <c r="G14" s="165">
         <v>0.20699999999999999</v>
       </c>
       <c r="H14" s="109">
@@ -4140,8 +4399,8 @@
       <c r="N14" s="15"/>
     </row>
     <row r="15" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="166"/>
-      <c r="C15" s="175"/>
+      <c r="B15" s="199"/>
+      <c r="C15" s="208"/>
       <c r="D15" s="12" t="s">
         <v>4</v>
       </c>
@@ -4161,7 +4420,7 @@
       <c r="J15" s="97">
         <v>0.13900000000000001</v>
       </c>
-      <c r="K15" s="192">
+      <c r="K15" s="172">
         <v>-0.317</v>
       </c>
       <c r="L15" s="138">
@@ -4170,8 +4429,8 @@
       <c r="M15" s="3"/>
     </row>
     <row r="16" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="166"/>
-      <c r="C16" s="176"/>
+      <c r="B16" s="199"/>
+      <c r="C16" s="209"/>
       <c r="D16" s="14" t="s">
         <v>5</v>
       </c>
@@ -4194,7 +4453,7 @@
       <c r="K16" s="103">
         <v>-0.72299999999999998</v>
       </c>
-      <c r="L16" s="195">
+      <c r="L16" s="175">
         <v>-4.2000000000000003E-2</v>
       </c>
       <c r="M16" s="3"/>
@@ -4213,10 +4472,10 @@
       <c r="L17" s="24"/>
     </row>
     <row r="18" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="165" t="s">
+      <c r="B18" s="198" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="174" t="s">
+      <c r="C18" s="211" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="50" t="s">
@@ -4232,8 +4491,8 @@
       <c r="L18" s="95"/>
     </row>
     <row r="19" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="166"/>
-      <c r="C19" s="175"/>
+      <c r="B19" s="199"/>
+      <c r="C19" s="208"/>
       <c r="D19" s="49" t="s">
         <v>9</v>
       </c>
@@ -4247,8 +4506,8 @@
       <c r="L19" s="96"/>
     </row>
     <row r="20" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="166"/>
-      <c r="C20" s="175"/>
+      <c r="B20" s="199"/>
+      <c r="C20" s="208"/>
       <c r="D20" s="49" t="s">
         <v>2</v>
       </c>
@@ -4262,8 +4521,8 @@
       <c r="L20" s="97"/>
     </row>
     <row r="21" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="166"/>
-      <c r="C21" s="175"/>
+      <c r="B21" s="199"/>
+      <c r="C21" s="208"/>
       <c r="D21" s="13" t="s">
         <v>3</v>
       </c>
@@ -4277,8 +4536,8 @@
       <c r="L21" s="97"/>
     </row>
     <row r="22" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="166"/>
-      <c r="C22" s="175"/>
+      <c r="B22" s="199"/>
+      <c r="C22" s="208"/>
       <c r="D22" s="12" t="s">
         <v>4</v>
       </c>
@@ -4292,8 +4551,8 @@
       <c r="L22" s="97"/>
     </row>
     <row r="23" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="166"/>
-      <c r="C23" s="176"/>
+      <c r="B23" s="199"/>
+      <c r="C23" s="209"/>
       <c r="D23" s="14" t="s">
         <v>5</v>
       </c>
@@ -4307,8 +4566,8 @@
       <c r="L23" s="98"/>
     </row>
     <row r="24" spans="2:14" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="166"/>
-      <c r="C24" s="177" t="s">
+      <c r="B24" s="199"/>
+      <c r="C24" s="210" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="13" t="s">
@@ -4326,8 +4585,8 @@
       <c r="N24" s="15"/>
     </row>
     <row r="25" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="166"/>
-      <c r="C25" s="175"/>
+      <c r="B25" s="199"/>
+      <c r="C25" s="208"/>
       <c r="D25" s="12" t="s">
         <v>9</v>
       </c>
@@ -4341,8 +4600,8 @@
       <c r="L25" s="96"/>
     </row>
     <row r="26" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="166"/>
-      <c r="C26" s="175"/>
+      <c r="B26" s="199"/>
+      <c r="C26" s="208"/>
       <c r="D26" s="13" t="s">
         <v>2</v>
       </c>
@@ -4357,8 +4616,8 @@
       <c r="M26" s="15"/>
     </row>
     <row r="27" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="166"/>
-      <c r="C27" s="175"/>
+      <c r="B27" s="199"/>
+      <c r="C27" s="208"/>
       <c r="D27" s="12" t="s">
         <v>3</v>
       </c>
@@ -4373,8 +4632,8 @@
       <c r="N27" s="15"/>
     </row>
     <row r="28" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="166"/>
-      <c r="C28" s="175"/>
+      <c r="B28" s="199"/>
+      <c r="C28" s="208"/>
       <c r="D28" s="12" t="s">
         <v>4</v>
       </c>
@@ -4388,8 +4647,8 @@
       <c r="L28" s="97"/>
     </row>
     <row r="29" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="166"/>
-      <c r="C29" s="176"/>
+      <c r="B29" s="199"/>
+      <c r="C29" s="209"/>
       <c r="D29" s="14" t="s">
         <v>5</v>
       </c>
@@ -4416,10 +4675,10 @@
       <c r="L30" s="21"/>
     </row>
     <row r="31" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="165" t="s">
+      <c r="B31" s="198" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="174" t="s">
+      <c r="C31" s="211" t="s">
         <v>0</v>
       </c>
       <c r="D31" s="25" t="s">
@@ -4435,8 +4694,8 @@
       <c r="L31" s="123"/>
     </row>
     <row r="32" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="166"/>
-      <c r="C32" s="175"/>
+      <c r="B32" s="199"/>
+      <c r="C32" s="208"/>
       <c r="D32" s="7" t="s">
         <v>9</v>
       </c>
@@ -4450,8 +4709,8 @@
       <c r="L32" s="85"/>
     </row>
     <row r="33" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="166"/>
-      <c r="C33" s="175"/>
+      <c r="B33" s="199"/>
+      <c r="C33" s="208"/>
       <c r="D33" s="8" t="s">
         <v>2</v>
       </c>
@@ -4465,8 +4724,8 @@
       <c r="L33" s="124"/>
     </row>
     <row r="34" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="166"/>
-      <c r="C34" s="175"/>
+      <c r="B34" s="199"/>
+      <c r="C34" s="208"/>
       <c r="D34" s="7" t="s">
         <v>3</v>
       </c>
@@ -4480,8 +4739,8 @@
       <c r="L34" s="125"/>
     </row>
     <row r="35" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="166"/>
-      <c r="C35" s="175"/>
+      <c r="B35" s="199"/>
+      <c r="C35" s="208"/>
       <c r="D35" s="7" t="s">
         <v>4</v>
       </c>
@@ -4495,8 +4754,8 @@
       <c r="L35" s="125"/>
     </row>
     <row r="36" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="166"/>
-      <c r="C36" s="176"/>
+      <c r="B36" s="199"/>
+      <c r="C36" s="209"/>
       <c r="D36" s="9" t="s">
         <v>5</v>
       </c>
@@ -4510,8 +4769,8 @@
       <c r="L36" s="127"/>
     </row>
     <row r="37" spans="2:14" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="166"/>
-      <c r="C37" s="177" t="s">
+      <c r="B37" s="199"/>
+      <c r="C37" s="210" t="s">
         <v>1</v>
       </c>
       <c r="D37" s="8" t="s">
@@ -4527,8 +4786,8 @@
       <c r="L37" s="81"/>
     </row>
     <row r="38" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="166"/>
-      <c r="C38" s="175"/>
+      <c r="B38" s="199"/>
+      <c r="C38" s="208"/>
       <c r="D38" s="7" t="s">
         <v>9</v>
       </c>
@@ -4542,8 +4801,8 @@
       <c r="L38" s="85"/>
     </row>
     <row r="39" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="166"/>
-      <c r="C39" s="175"/>
+      <c r="B39" s="199"/>
+      <c r="C39" s="208"/>
       <c r="D39" s="8" t="s">
         <v>2</v>
       </c>
@@ -4558,8 +4817,8 @@
       <c r="N39" s="15"/>
     </row>
     <row r="40" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="166"/>
-      <c r="C40" s="175"/>
+      <c r="B40" s="199"/>
+      <c r="C40" s="208"/>
       <c r="D40" s="7" t="s">
         <v>3</v>
       </c>
@@ -4573,8 +4832,8 @@
       <c r="L40" s="125"/>
     </row>
     <row r="41" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="166"/>
-      <c r="C41" s="175"/>
+      <c r="B41" s="199"/>
+      <c r="C41" s="208"/>
       <c r="D41" s="7" t="s">
         <v>4</v>
       </c>
@@ -4589,8 +4848,8 @@
       <c r="N41" s="15"/>
     </row>
     <row r="42" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="167"/>
-      <c r="C42" s="178"/>
+      <c r="B42" s="200"/>
+      <c r="C42" s="212"/>
       <c r="D42" s="22" t="s">
         <v>5</v>
       </c>
@@ -4701,6 +4960,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B18:B29"/>
+    <mergeCell ref="C18:C23"/>
+    <mergeCell ref="C24:C29"/>
+    <mergeCell ref="B31:B42"/>
+    <mergeCell ref="C31:C36"/>
+    <mergeCell ref="C37:C42"/>
     <mergeCell ref="B5:B16"/>
     <mergeCell ref="C5:C10"/>
     <mergeCell ref="C11:C16"/>
@@ -4709,12 +4974,6 @@
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
-    <mergeCell ref="B18:B29"/>
-    <mergeCell ref="C18:C23"/>
-    <mergeCell ref="C24:C29"/>
-    <mergeCell ref="B31:B42"/>
-    <mergeCell ref="C31:C36"/>
-    <mergeCell ref="C37:C42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4723,10 +4982,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19302950-C106-4780-AFCB-B595BCCB0D58}">
-  <dimension ref="B1:M31"/>
+  <dimension ref="B1:T33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScaleSheetLayoutView="50" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4734,14 +4993,14 @@
     <col min="1" max="1" width="8.42578125" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
     <col min="5" max="8" width="7.140625" customWidth="1"/>
     <col min="9" max="9" width="6.85546875" customWidth="1"/>
     <col min="10" max="10" width="7.42578125" customWidth="1"/>
     <col min="11" max="11" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:20" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
       <c r="D1" s="53"/>
@@ -4751,7 +5010,7 @@
       <c r="H1" s="56"/>
       <c r="I1" s="59"/>
     </row>
-    <row r="2" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:20" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2"/>
@@ -4760,36 +5019,36 @@
       <c r="G2"/>
       <c r="H2"/>
     </row>
-    <row r="3" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:20" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3"/>
       <c r="C3"/>
       <c r="D3"/>
-      <c r="E3" s="161" t="s">
+      <c r="E3" s="194" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="162"/>
-      <c r="G3" s="162"/>
-      <c r="H3" s="163"/>
-      <c r="I3" s="164" t="s">
+      <c r="F3" s="195"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="196"/>
+      <c r="I3" s="197" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="162"/>
-      <c r="K3" s="163"/>
-    </row>
-    <row r="4" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="171" t="s">
+      <c r="J3" s="195"/>
+      <c r="K3" s="196"/>
+    </row>
+    <row r="4" spans="2:20" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="204" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="172"/>
-      <c r="D4" s="173"/>
-      <c r="E4" s="168" t="s">
+      <c r="C4" s="205"/>
+      <c r="D4" s="206"/>
+      <c r="E4" s="201" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="169"/>
-      <c r="G4" s="170" t="s">
+      <c r="F4" s="202"/>
+      <c r="G4" s="203" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="169"/>
+      <c r="H4" s="202"/>
       <c r="I4" s="28" t="s">
         <v>21</v>
       </c>
@@ -4800,292 +5059,394 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:20" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="228" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="227" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="220" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="221" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="222" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="223" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="220" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="223" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="223" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="179" t="s">
+    <row r="6" spans="2:20" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="219" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="181" t="s">
+      <c r="C6" s="217" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="220">
+      <c r="E6" s="226">
         <v>0.63100000000000001</v>
       </c>
-      <c r="F6" s="212">
+      <c r="F6" s="268">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G6" s="110">
+      <c r="G6" s="241">
         <v>0.216</v>
       </c>
-      <c r="H6" s="221">
+      <c r="H6" s="270">
         <v>0.45</v>
       </c>
-      <c r="I6" s="228">
+      <c r="I6" s="245">
         <v>0.17799999999999999</v>
       </c>
-      <c r="J6" s="226">
+      <c r="J6" s="191">
         <v>-0.39500000000000002</v>
       </c>
-      <c r="K6" s="222">
+      <c r="K6" s="249">
         <v>-5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="180"/>
-      <c r="C7" s="182"/>
-      <c r="D7" s="52" t="s">
+    <row r="7" spans="2:20" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="213"/>
+      <c r="C7" s="218"/>
+      <c r="D7" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="140">
+      <c r="E7" s="117">
         <v>0.63500000000000001</v>
       </c>
-      <c r="F7" s="227">
+      <c r="F7" s="269">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G7" s="211">
+      <c r="G7" s="229">
         <v>0.21099999999999999</v>
       </c>
-      <c r="H7" s="227">
+      <c r="H7" s="269">
         <v>0.45</v>
       </c>
-      <c r="I7" s="225">
+      <c r="I7" s="246">
         <v>0.19900000000000001</v>
       </c>
-      <c r="J7" s="229">
+      <c r="J7" s="272">
         <v>-6.9099999999999995E-2</v>
       </c>
-      <c r="K7" s="236">
+      <c r="K7" s="250">
         <v>-0.115</v>
       </c>
     </row>
-    <row r="8" spans="2:13" s="57" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="152"/>
-      <c r="C8" s="153"/>
-      <c r="D8" s="154"/>
-      <c r="E8" s="155"/>
-      <c r="F8" s="156"/>
-      <c r="G8" s="157"/>
-      <c r="H8" s="156"/>
-      <c r="I8" s="158"/>
-      <c r="J8" s="159"/>
-      <c r="K8" s="160"/>
-    </row>
-    <row r="9" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="179" t="s">
+    <row r="8" spans="2:20" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="213"/>
+      <c r="C8" s="231"/>
+      <c r="D8" s="264" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="265">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="F8" s="240">
+        <v>1.23</v>
+      </c>
+      <c r="G8" s="266">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="H8" s="240">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="247">
+        <v>0.185</v>
+      </c>
+      <c r="J8" s="267">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="K8" s="251">
+        <v>-0.14099999999999999</v>
+      </c>
+      <c r="L8" s="230" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" s="57" customFormat="1" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="161"/>
+      <c r="C9" s="162" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="243">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="F9" s="244">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G9" s="276">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="H9" s="119">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="I9" s="271">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="J9" s="128">
+        <v>-0.69799999999999995</v>
+      </c>
+      <c r="K9" s="263">
+        <v>-4.7899999999999998E-2</v>
+      </c>
+      <c r="M9" s="234"/>
+      <c r="N9" s="234"/>
+      <c r="O9" s="234"/>
+      <c r="P9" s="234"/>
+      <c r="Q9" s="234"/>
+      <c r="R9" s="234"/>
+      <c r="S9" s="234"/>
+      <c r="T9" s="234"/>
+    </row>
+    <row r="10" spans="2:20" s="57" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="152"/>
+      <c r="C10" s="153"/>
+      <c r="D10" s="154"/>
+      <c r="E10" s="155"/>
+      <c r="F10" s="156"/>
+      <c r="G10" s="157"/>
+      <c r="H10" s="156"/>
+      <c r="I10" s="158"/>
+      <c r="J10" s="159"/>
+      <c r="K10" s="160"/>
+      <c r="M10" s="234"/>
+      <c r="N10" s="234"/>
+      <c r="O10" s="234"/>
+      <c r="P10" s="234"/>
+      <c r="Q10" s="234"/>
+      <c r="R10" s="234"/>
+      <c r="S10" s="234"/>
+      <c r="T10" s="234"/>
+    </row>
+    <row r="11" spans="2:20" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="213" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="181" t="s">
+      <c r="C11" s="215" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="130"/>
-      <c r="F9" s="131"/>
-      <c r="G9" s="139"/>
-      <c r="H9" s="131"/>
-      <c r="I9" s="149"/>
-      <c r="J9" s="150"/>
-      <c r="K9" s="151"/>
-      <c r="L9" s="61"/>
-      <c r="M9"/>
-    </row>
-    <row r="10" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="180"/>
-      <c r="C10" s="182"/>
-      <c r="D10" s="52" t="s">
+      <c r="E11" s="130"/>
+      <c r="F11" s="131"/>
+      <c r="G11" s="139"/>
+      <c r="H11" s="131"/>
+      <c r="I11" s="149"/>
+      <c r="J11" s="150"/>
+      <c r="K11" s="151"/>
+      <c r="L11" s="61"/>
+      <c r="M11" s="234"/>
+      <c r="N11" s="234"/>
+      <c r="O11" s="234"/>
+      <c r="P11" s="234"/>
+      <c r="Q11" s="234"/>
+      <c r="R11" s="234"/>
+      <c r="S11" s="234"/>
+      <c r="T11" s="234"/>
+    </row>
+    <row r="12" spans="2:20" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="214"/>
+      <c r="C12" s="216"/>
+      <c r="D12" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="140"/>
-      <c r="F10" s="141"/>
-      <c r="G10" s="142"/>
-      <c r="H10" s="141"/>
-      <c r="I10" s="143"/>
-      <c r="J10" s="144"/>
-      <c r="K10" s="145"/>
-      <c r="L10" s="61"/>
-      <c r="M10"/>
-    </row>
-    <row r="11" spans="2:13" s="57" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="152"/>
-      <c r="C11" s="153"/>
-      <c r="D11" s="154"/>
-      <c r="E11" s="155"/>
-      <c r="F11" s="156"/>
-      <c r="G11" s="157"/>
-      <c r="H11" s="156"/>
-      <c r="I11" s="158"/>
-      <c r="J11" s="159"/>
-      <c r="K11" s="160"/>
-      <c r="L11" s="61"/>
-      <c r="M11"/>
-    </row>
-    <row r="12" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="179" t="s">
+      <c r="E12" s="140"/>
+      <c r="F12" s="141"/>
+      <c r="G12" s="142"/>
+      <c r="H12" s="141"/>
+      <c r="I12" s="143"/>
+      <c r="J12" s="144"/>
+      <c r="K12" s="145"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="235"/>
+      <c r="N12" s="235"/>
+      <c r="O12" s="236"/>
+      <c r="P12" s="237"/>
+      <c r="Q12" s="236"/>
+      <c r="R12" s="236"/>
+      <c r="S12" s="237"/>
+      <c r="T12" s="234"/>
+    </row>
+    <row r="13" spans="2:20" s="57" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="152"/>
+      <c r="C13" s="153"/>
+      <c r="D13" s="154"/>
+      <c r="E13" s="155"/>
+      <c r="F13" s="156"/>
+      <c r="G13" s="157"/>
+      <c r="H13" s="156"/>
+      <c r="I13" s="158"/>
+      <c r="J13" s="159"/>
+      <c r="K13" s="160"/>
+      <c r="L13" s="61"/>
+      <c r="M13" s="234"/>
+      <c r="N13" s="234"/>
+      <c r="O13" s="234"/>
+      <c r="P13" s="234"/>
+      <c r="Q13" s="234"/>
+      <c r="R13" s="234"/>
+      <c r="S13" s="234"/>
+      <c r="T13" s="234"/>
+    </row>
+    <row r="14" spans="2:20" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="213" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="181" t="s">
+      <c r="C14" s="215" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D14" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="130"/>
-      <c r="F12" s="131"/>
-      <c r="G12" s="139"/>
-      <c r="H12" s="131"/>
-      <c r="I12" s="146"/>
-      <c r="J12" s="147"/>
-      <c r="K12" s="148"/>
-      <c r="L12"/>
-      <c r="M12"/>
-    </row>
-    <row r="13" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="180"/>
-      <c r="C13" s="182"/>
-      <c r="D13" s="52" t="s">
+      <c r="E14" s="130"/>
+      <c r="F14" s="131"/>
+      <c r="G14" s="139"/>
+      <c r="H14" s="131"/>
+      <c r="I14" s="146"/>
+      <c r="J14" s="147"/>
+      <c r="K14" s="148"/>
+      <c r="L14"/>
+      <c r="M14" s="234"/>
+      <c r="N14" s="234"/>
+      <c r="O14" s="234"/>
+      <c r="P14" s="234"/>
+      <c r="Q14" s="234"/>
+      <c r="R14" s="234"/>
+      <c r="S14" s="234"/>
+      <c r="T14" s="234"/>
+    </row>
+    <row r="15" spans="2:20" s="57" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="214"/>
+      <c r="C15" s="216"/>
+      <c r="D15" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="140"/>
-      <c r="F13" s="141"/>
-      <c r="G13" s="142"/>
-      <c r="H13" s="141"/>
-      <c r="I13" s="143"/>
-      <c r="J13" s="144"/>
-      <c r="K13" s="145"/>
-      <c r="L13"/>
-      <c r="M13"/>
-    </row>
-    <row r="14" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="58"/>
-    </row>
-    <row r="15" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="56"/>
-    </row>
-    <row r="16" spans="2:13" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E15" s="140"/>
+      <c r="F15" s="141"/>
+      <c r="G15" s="142"/>
+      <c r="H15" s="141"/>
+      <c r="I15" s="143"/>
+      <c r="J15" s="144"/>
+      <c r="K15" s="145"/>
+      <c r="L15"/>
+      <c r="M15" s="234"/>
+      <c r="N15" s="234"/>
+      <c r="O15" s="234"/>
+      <c r="P15" s="234"/>
+      <c r="Q15" s="234"/>
+      <c r="R15" s="234"/>
+      <c r="S15" s="234"/>
+      <c r="T15" s="234"/>
+    </row>
+    <row r="16" spans="2:20" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="60"/>
       <c r="C16" s="60"/>
       <c r="D16" s="53"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+      <c r="M16" s="234"/>
+      <c r="N16" s="234"/>
+      <c r="O16" s="234"/>
+      <c r="P16" s="234"/>
+      <c r="Q16" s="234"/>
+      <c r="R16" s="234"/>
+      <c r="S16" s="234"/>
+      <c r="T16" s="234"/>
     </row>
     <row r="17" spans="2:12" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="60"/>
-      <c r="C17" s="223"/>
-      <c r="D17" s="224"/>
-      <c r="E17" s="202"/>
-      <c r="F17" s="202"/>
-      <c r="G17" s="202"/>
-      <c r="H17" s="202"/>
-      <c r="I17" s="203"/>
-      <c r="J17" s="203"/>
-      <c r="K17" s="203"/>
-      <c r="L17" s="203"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="56"/>
     </row>
     <row r="18" spans="2:12" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="60"/>
-      <c r="C18" s="223"/>
-      <c r="D18" s="224"/>
-      <c r="E18" s="201"/>
-      <c r="F18" s="202"/>
-      <c r="G18" s="201"/>
-      <c r="H18" s="202"/>
-      <c r="I18" s="204"/>
-      <c r="J18" s="203"/>
-      <c r="K18" s="203"/>
-      <c r="L18" s="203"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
     </row>
     <row r="19" spans="2:12" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="60"/>
-      <c r="C19" s="223"/>
-      <c r="D19" s="200"/>
-      <c r="E19" s="200"/>
-      <c r="F19" s="201"/>
-      <c r="G19" s="202"/>
-      <c r="H19" s="202"/>
-      <c r="I19" s="201"/>
-      <c r="J19" s="201"/>
-      <c r="K19" s="201"/>
-      <c r="L19" s="203"/>
+      <c r="C19" s="189"/>
+      <c r="D19" s="190"/>
+      <c r="E19" s="180"/>
+      <c r="F19" s="180"/>
+      <c r="G19" s="180"/>
+      <c r="H19" s="180"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
     </row>
     <row r="20" spans="2:12" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="60"/>
-      <c r="C20" s="223"/>
-      <c r="D20" s="224"/>
-      <c r="E20" s="200"/>
-      <c r="F20" s="200"/>
-      <c r="G20" s="201"/>
-      <c r="H20" s="202"/>
-      <c r="I20" s="204"/>
-      <c r="J20" s="203"/>
-      <c r="K20" s="203"/>
-      <c r="L20" s="203"/>
+      <c r="C20" s="189"/>
+      <c r="D20" s="190"/>
+      <c r="E20" s="112"/>
+      <c r="F20" s="180"/>
+      <c r="G20" s="112"/>
+      <c r="H20" s="180"/>
+      <c r="I20" s="15"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
     </row>
     <row r="21" spans="2:12" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="60"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="56"/>
+      <c r="C21" s="189"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="112"/>
+      <c r="G21" s="180"/>
+      <c r="H21" s="180"/>
+      <c r="I21" s="112"/>
+      <c r="J21" s="112"/>
+      <c r="K21" s="112"/>
+      <c r="L21"/>
     </row>
     <row r="22" spans="2:12" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="60"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="56"/>
+      <c r="C22" s="189"/>
+      <c r="D22" s="190"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="112"/>
+      <c r="H22" s="180"/>
+      <c r="I22" s="15"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
     </row>
     <row r="23" spans="2:12" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="60"/>
@@ -5093,7 +5454,7 @@
       <c r="D23" s="53"/>
       <c r="E23" s="54"/>
       <c r="F23" s="55"/>
-      <c r="G23" s="56"/>
+      <c r="G23" s="58"/>
       <c r="H23" s="56"/>
     </row>
     <row r="24" spans="2:12" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5102,7 +5463,7 @@
       <c r="D24" s="53"/>
       <c r="E24" s="54"/>
       <c r="F24" s="55"/>
-      <c r="G24" s="58"/>
+      <c r="G24" s="56"/>
       <c r="H24" s="56"/>
     </row>
     <row r="25" spans="2:12" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5111,7 +5472,7 @@
       <c r="D25" s="53"/>
       <c r="E25" s="54"/>
       <c r="F25" s="55"/>
-      <c r="G25" s="58"/>
+      <c r="G25" s="56"/>
       <c r="H25" s="56"/>
     </row>
     <row r="26" spans="2:12" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5121,7 +5482,7 @@
       <c r="E26" s="54"/>
       <c r="F26" s="55"/>
       <c r="G26" s="58"/>
-      <c r="H26" s="58"/>
+      <c r="H26" s="56"/>
     </row>
     <row r="27" spans="2:12" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="60"/>
@@ -5132,23 +5493,41 @@
       <c r="G27" s="58"/>
       <c r="H27" s="56"/>
     </row>
-    <row r="28" spans="2:12" s="57" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:12" s="57" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:12" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="60"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="58"/>
+    </row>
+    <row r="29" spans="2:12" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="60"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="56"/>
+    </row>
     <row r="30" spans="2:12" s="57" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="2:12" s="57" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:12" s="57" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="57" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B6:B8"/>
     <mergeCell ref="I3:K3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="E3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5156,12 +5535,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A69AE6C51AEE6142AD84D9FB7E253133" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="688ae3312de6a1cdf808e1735a79ca91">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="756e89ea-a5fb-4d06-a9be-9b8635efcbbf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7ae5de413dc6742d84d7e8ba9b183640" ns3:_="">
     <xsd:import namespace="756e89ea-a5fb-4d06-a9be-9b8635efcbbf"/>
@@ -5337,6 +5710,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5347,22 +5726,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A6A8E2B-A170-438C-86CD-560003D30CAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="756e89ea-a5fb-4d06-a9be-9b8635efcbbf"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F55020E-069C-4126-815D-85E5FA260EED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5380,6 +5743,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A6A8E2B-A170-438C-86CD-560003D30CAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="756e89ea-a5fb-4d06-a9be-9b8635efcbbf"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06DA2F1B-717B-4D32-8536-28EBD29FAA3A}">
   <ds:schemaRefs>

</xml_diff>